<commit_message>
Iteration 2, Projekt, Updaterat Vision & Kravspec
</commit_message>
<xml_diff>
--- a/Dokumentation/Iteration v16/Iteration1.xlsx
+++ b/Dokumentation/Iteration v16/Iteration1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>Analys av föregående iteration</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Studering av XNA</t>
+  </si>
+  <si>
+    <t>Ej klart</t>
   </si>
 </sst>
 </file>
@@ -172,9 +175,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -185,6 +185,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B31:B32"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,20 +523,20 @@
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -541,124 +544,124 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>3</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>1</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>3</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>6</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5" t="s">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>13</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>8</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4">
         <v>240</v>
       </c>
     </row>
@@ -668,152 +671,166 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
     </row>
     <row r="19" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="4">
+        <v>6</v>
+      </c>
+      <c r="E22" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="4">
+        <v>6</v>
+      </c>
+      <c r="E23" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E24" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D25" s="6">
+        <v>4</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="4">
+        <v>3</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="4">
         <v>6</v>
       </c>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="5">
+      <c r="E27" s="4">
         <v>6</v>
       </c>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="7">
-        <v>4</v>
-      </c>
-      <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="5" t="s">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="4">
+        <v>26.5</v>
+      </c>
+      <c r="E28" s="4">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="4">
+        <v>21</v>
+      </c>
+      <c r="E29" s="4">
         <v>25</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="5">
-        <v>3</v>
-      </c>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="5">
-        <v>6</v>
-      </c>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="5">
-        <v>26.5</v>
-      </c>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="5">
-        <v>21</v>
-      </c>
-      <c r="E29" s="5">
-        <v>25</v>
-      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5" t="s">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5">
+      <c r="D30" s="4"/>
+      <c r="E30" s="4">
         <v>240</v>
       </c>
     </row>

</xml_diff>